<commit_message>
update in formula for validation
</commit_message>
<xml_diff>
--- a/fms_core/static/submission_templates/Sample_submission_v0.5.xlsx
+++ b/fms_core/static/submission_templates/Sample_submission_v0.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kseni\Documents\fms\fms_core\static\submission_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CCE429-A3B9-4773-8D13-402ED2052E93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107665F4-FEA1-43E9-95A3-90CF2658148B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1710,7 +1710,7 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1966,7 +1966,7 @@
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
-      <c r="L11" s="9"/>
+      <c r="L11" s="11"/>
       <c r="M11" s="10"/>
       <c r="N11" s="11"/>
       <c r="O11" s="10"/>
@@ -17510,12 +17510,6 @@
             <xm:f>Index!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>G8:G391</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Coordinate" xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>IF(OR(H8="Tube",H8="Plate96"),Index!$A$2:$A$97,IF(H8="Plate384",Index!$B$2:$B$385,""))</xm:f>
-          </x14:formula1>
-          <xm:sqref>L8:L391</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C4AE9989-C53C-4620-8311-6243A0036F42}">
           <x14:formula1>
@@ -17540,6 +17534,12 @@
             <xm:f>Index!$F$2:$F$4</xm:f>
           </x14:formula1>
           <xm:sqref>T8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Coordinate" xr:uid="{BC1B1449-32C7-49D5-8D49-9DE1F0C24D5A}">
+          <x14:formula1>
+            <xm:f>IF(OR(H8="Tube",H8="96-well plate"),Index!$A$2:$A$97,IF(H8="384-well plate",Index!$B$2:$B$385,""))</xm:f>
+          </x14:formula1>
+          <xm:sqref>L8:L391</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>